<commit_message>
Icon seg final model
</commit_message>
<xml_diff>
--- a/cityscapes/regular_multi_modal_classification_report.xlsx
+++ b/cityscapes/regular_multi_modal_classification_report.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9271594212777341</v>
+        <v>0.9301554646195587</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6026443811811145</v>
+        <v>0.6058669934699258</v>
       </c>
       <c r="D2" t="n">
-        <v>0.730482451140581</v>
+        <v>0.7337789780881485</v>
       </c>
       <c r="E2" t="n">
         <v>2392469</v>
@@ -481,13 +481,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8254146236927344</v>
+        <v>0.8686266612010792</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9553837968799129</v>
+        <v>0.9465721429073342</v>
       </c>
       <c r="D3" t="n">
-        <v>0.885656397797326</v>
+        <v>0.9059258944183849</v>
       </c>
       <c r="E3" t="n">
         <v>6176366</v>
@@ -500,13 +500,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5060196671969941</v>
+        <v>0.5800353423767848</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3894319705458499</v>
+        <v>0.5509822308055513</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4401359667579778</v>
+        <v>0.5651356344350986</v>
       </c>
       <c r="E4" t="n">
         <v>1056829</v>
@@ -519,13 +519,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7173396125185207</v>
+        <v>0.6801786589471244</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8167396982142986</v>
+        <v>0.9011592962120328</v>
       </c>
       <c r="D5" t="n">
-        <v>0.76381935998559</v>
+        <v>0.7752287480300734</v>
       </c>
       <c r="E5" t="n">
         <v>3873212</v>
@@ -557,13 +557,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>0.06289308176100629</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.0001186394428691763</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.0002368321333838575</v>
       </c>
       <c r="E7" t="n">
         <v>168578</v>
@@ -576,13 +576,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>0.4716636197440585</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.001205584942337526</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.00240502258204343</v>
       </c>
       <c r="E8" t="n">
         <v>214004</v>
@@ -633,13 +633,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.6992848414951393</v>
+        <v>0.7865976375601036</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8282395123752746</v>
+        <v>0.7297303430583276</v>
       </c>
       <c r="D11" t="n">
-        <v>0.758318955326442</v>
+        <v>0.7570976348685434</v>
       </c>
       <c r="E11" t="n">
         <v>2732101</v>
@@ -652,13 +652,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.09539052496798976</v>
+        <v>0.2425787019606707</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0007398763562330859</v>
+        <v>0.04159197556918341</v>
       </c>
       <c r="D12" t="n">
-        <v>0.001468363661448556</v>
+        <v>0.07100892698186628</v>
       </c>
       <c r="E12" t="n">
         <v>201385</v>
@@ -671,13 +671,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.8604401663553559</v>
+        <v>0.8792954453401336</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8978337562942381</v>
+        <v>0.8940070379505203</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8787393325621494</v>
+        <v>0.8865902168175908</v>
       </c>
       <c r="E13" t="n">
         <v>672639</v>
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.245433103639643</v>
+        <v>0.3403777526329533</v>
       </c>
       <c r="C14" t="n">
-        <v>0.02246634493268987</v>
+        <v>0.1655490644314622</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04116458465034924</v>
+        <v>0.2227564011278517</v>
       </c>
       <c r="E14" t="n">
         <v>236220</v>
@@ -728,13 +728,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6301215595586225</v>
+        <v>0.6240941177056816</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7991041480380674</v>
+        <v>0.8412528493885622</v>
       </c>
       <c r="D16" t="n">
-        <v>0.7046231387178521</v>
+        <v>0.7165824430614578</v>
       </c>
       <c r="E16" t="n">
         <v>1191045</v>
@@ -842,16 +842,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.759926563984639</v>
+        <v>0.7739371222418707</v>
       </c>
       <c r="C22" t="n">
-        <v>0.759926563984639</v>
+        <v>0.7739371222418707</v>
       </c>
       <c r="D22" t="n">
-        <v>0.759926563984639</v>
+        <v>0.7739371222418707</v>
       </c>
       <c r="E22" t="n">
-        <v>0.759926563984639</v>
+        <v>0.7739371222418707</v>
       </c>
     </row>
     <row r="23">
@@ -861,13 +861,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.2753301760351367</v>
+        <v>0.3233248241924577</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2656291742408839</v>
+        <v>0.2839018079089053</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2602204275299858</v>
+        <v>0.2818373366272222</v>
       </c>
       <c r="E23" t="n">
         <v>19398656</v>
@@ -880,13 +880,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.7189374168291598</v>
+        <v>0.7506928016837868</v>
       </c>
       <c r="C24" t="n">
-        <v>0.759926563984639</v>
+        <v>0.7739371222418707</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7296130845309581</v>
+        <v>0.7493575289337119</v>
       </c>
       <c r="E24" t="n">
         <v>19398656</v>

</xml_diff>